<commit_message>
fixed x axis values
</commit_message>
<xml_diff>
--- a/GameEngine/Assignment1revisited.xlsx
+++ b/GameEngine/Assignment1revisited.xlsx
@@ -200,10 +200,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scenario1!$A$2:$A$9</c:f>
+              <c:f>Scenario1!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -227,16 +227,88 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenario1!$B$2:$B$9</c:f>
+              <c:f>Scenario1!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>6.9206339999999997</c:v>
                 </c:pt>
@@ -260,6 +332,78 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9.6431780000000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.020083</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.429066000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.906212999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.299158</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.760266</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.173259</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.510068</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.870936</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.316005000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.829238999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.302376000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.971985</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.376958999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.397007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15.749855</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16.206954</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15.58947</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15.661643</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16.018501000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16.35932</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16.744244999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17.189315000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.542162999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17.907039999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -294,10 +438,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scenario1!$A$2:$A$9</c:f>
+              <c:f>Scenario1!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -321,16 +465,88 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenario1!$C$2:$C$9</c:f>
+              <c:f>Scenario1!$C$2:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>13.528516</c:v>
                 </c:pt>
@@ -354,6 +570,78 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>63.472557999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>69.017886000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72.217575999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>74.302588</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79.871973999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.345129</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90.557657000000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96.006754000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100.97870399999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>110.718113</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>115.846439</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121.247421</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>124.996431</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>130.441519</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>137.15365199999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>142.45038199999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>147.90348900000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>153.27640299999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>158.516999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>166.09922299999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>171.51223300000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>176.68867499999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>185.634175</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>189.094492</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>195.37759399999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -786,10 +1074,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scenario2!$A$2:$A$9</c:f>
+              <c:f>Scenario2!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -813,16 +1101,88 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenario2!$B$2:$B$9</c:f>
+              <c:f>Scenario2!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>322.27860299999998</c:v>
                 </c:pt>
@@ -846,6 +1206,78 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2577.9281019999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2846.7261629999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3160.1835639999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3460.6497410000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3769.5161069999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4079.3848830000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4404.5023090000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4714.8362029999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5021.0562090000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5325.8447740000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5666.2308990000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5970.7387900000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6300.9404359999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6601.0537649999997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6914.9762840000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7219.4881839999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7531.3216819999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7866.3950379999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8167.1258500000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8484.8615339999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8800.6365060000007</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9115.8060220000007</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9444.2153610000005</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9763.7112749999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10067.381152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -880,10 +1312,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Scenario2!$A$2:$A$9</c:f>
+              <c:f>Scenario2!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -907,16 +1339,88 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Scenario2!$C$2:$C$9</c:f>
+              <c:f>Scenario2!$C$2:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>3530.7221610000001</c:v>
                 </c:pt>
@@ -940,6 +1444,78 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>26597.319189000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29005.258719000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31630.191799</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34355.718656999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36792.351152000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39379.156589999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42066.563826999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44725.041532000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47405.780742000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50719.914327999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>53260.095705</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>56796.050443</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>59532.074531999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>61957.219416</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>65276.260798000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>67973.395415000006</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>70649.695957000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>73320.703777999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>76060.829725000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>79445.749448000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>81899.863960999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>84617.752460000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>87248.635840999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>89900.088661000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>93743.482334999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2716,7 +3292,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,7 +3802,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Began thread safe testing of resource manager.
</commit_message>
<xml_diff>
--- a/GameEngine/Assignment1revisited.xlsx
+++ b/GameEngine/Assignment1revisited.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\GameEngine\GameEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\GE\GameEngine\GameEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario1" sheetId="1" r:id="rId1"/>
@@ -671,11 +671,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="267945232"/>
-        <c:axId val="267942488"/>
+        <c:axId val="237924392"/>
+        <c:axId val="237927920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="267945232"/>
+        <c:axId val="237924392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,7 +774,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267942488"/>
+        <c:crossAx val="237927920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -782,7 +782,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="267942488"/>
+        <c:axId val="237927920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +889,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267945232"/>
+        <c:crossAx val="237924392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1004,6 +1004,649 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scenario</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 1</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>Increase of speed-up</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.9702318460192481E-2"/>
+                  <c:y val="-0.15966681248177311"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Scenario1!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Scenario1!$D$2:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.9548087646305239</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9313020776121794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6366982545995254</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4329330423260771</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1443595324410198</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5462798339753139</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2545612032694899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5821203341885832</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8879555189313306</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.9246446421951866</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8128678579815016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0688430058239735</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.2570747124257222</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.43906434587484</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.6743590842192067</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.8454825663028691</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.314664420747814</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3769207401795587</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.4774320714264544</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.3486879662249187</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.4829203875746835</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.9078125378523243</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.0445519657165097</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.1259276110736174</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.8320470804972828</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.121351827518991</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.369211388756039</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.48406859209307</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.552203159951373</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.799393402238541</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10.779428511751943</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10.910658266246125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="400523768"/>
+        <c:axId val="235981728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="400523768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Allocations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sv-SE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="235981728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="235981728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Speed-up</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sv-SE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400523768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="sv-SE"/>
               <a:t>Scenario 2</a:t>
             </a:r>
@@ -1184,100 +1827,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>322.27860299999998</c:v>
+                  <c:v>0.322278603</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640.94051300000001</c:v>
+                  <c:v>0.64094051299999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>952.16454699999997</c:v>
+                  <c:v>0.95216454699999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1271.323652</c:v>
+                  <c:v>1.271323652</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1569.7890190000001</c:v>
+                  <c:v>1.5697890190000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1876.4460759999999</c:v>
+                  <c:v>1.8764460759999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2227.934886</c:v>
+                  <c:v>2.2279348859999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2577.9281019999999</c:v>
+                  <c:v>2.577928102</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2846.7261629999998</c:v>
+                  <c:v>2.846726163</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3160.1835639999999</c:v>
+                  <c:v>3.160183564</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3460.6497410000002</c:v>
+                  <c:v>3.4606497410000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3769.5161069999999</c:v>
+                  <c:v>3.7695161069999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4079.3848830000002</c:v>
+                  <c:v>4.0793848830000004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4404.5023090000004</c:v>
+                  <c:v>4.4045023090000006</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4714.8362029999998</c:v>
+                  <c:v>4.7148362029999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5021.0562090000003</c:v>
+                  <c:v>5.0210562090000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5325.8447740000001</c:v>
+                  <c:v>5.3258447740000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5666.2308990000001</c:v>
+                  <c:v>5.6662308990000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5970.7387900000003</c:v>
+                  <c:v>5.9707387900000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6300.9404359999999</c:v>
+                  <c:v>6.3009404359999994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6601.0537649999997</c:v>
+                  <c:v>6.6010537649999996</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6914.9762840000003</c:v>
+                  <c:v>6.9149762840000006</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7219.4881839999998</c:v>
+                  <c:v>7.2194881840000003</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7531.3216819999998</c:v>
+                  <c:v>7.5313216819999997</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7866.3950379999997</c:v>
+                  <c:v>7.8663950379999994</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8167.1258500000004</c:v>
+                  <c:v>8.1671258499999997</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8484.8615339999997</c:v>
+                  <c:v>8.4848615340000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8800.6365060000007</c:v>
+                  <c:v>8.800636506</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9115.8060220000007</c:v>
+                  <c:v>9.115806022000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9444.2153610000005</c:v>
+                  <c:v>9.4442153610000013</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9763.7112749999997</c:v>
+                  <c:v>9.7637112750000004</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10067.381152</c:v>
+                  <c:v>10.067381151999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1422,100 +2065,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>3530.7221610000001</c:v>
+                  <c:v>3.5307221610000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6969.8321310000001</c:v>
+                  <c:v>6.9698321310000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10034.23749</c:v>
+                  <c:v>10.034237489999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14177.940965</c:v>
+                  <c:v>14.177940964999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17029.566905</c:v>
+                  <c:v>17.029566904999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19802.443568999999</c:v>
+                  <c:v>19.802443568999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23832.718414999999</c:v>
+                  <c:v>23.832718414999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26597.319189000002</c:v>
+                  <c:v>26.597319189</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29005.258719000001</c:v>
+                  <c:v>29.005258719</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31630.191799</c:v>
+                  <c:v>31.630191798999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34355.718656999998</c:v>
+                  <c:v>34.355718656999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36792.351152000003</c:v>
+                  <c:v>36.792351152000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39379.156589999999</c:v>
+                  <c:v>39.379156590000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42066.563826999998</c:v>
+                  <c:v>42.066563826999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44725.041532000003</c:v>
+                  <c:v>44.725041532000006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>47405.780742000003</c:v>
+                  <c:v>47.405780742000005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50719.914327999999</c:v>
+                  <c:v>50.719914328000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>53260.095705</c:v>
+                  <c:v>53.260095704999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>56796.050443</c:v>
+                  <c:v>56.796050442999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>59532.074531999999</c:v>
+                  <c:v>59.532074531999996</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>61957.219416</c:v>
+                  <c:v>61.957219416000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>65276.260798000003</c:v>
+                  <c:v>65.27626079800001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>67973.395415000006</c:v>
+                  <c:v>67.973395415000013</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>70649.695957000004</c:v>
+                  <c:v>70.649695957000006</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>73320.703777999996</c:v>
+                  <c:v>73.320703777999995</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>76060.829725000003</c:v>
+                  <c:v>76.060829725000005</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>79445.749448000002</c:v>
+                  <c:v>79.445749448000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>81899.863960999995</c:v>
+                  <c:v>81.899863960999994</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>84617.752460000003</c:v>
+                  <c:v>84.617752460000005</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>87248.635840999996</c:v>
+                  <c:v>87.248635840999995</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>89900.088661000002</c:v>
+                  <c:v>89.900088660999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>93743.482334999993</c:v>
+                  <c:v>93.743482334999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1545,11 +2188,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="267944448"/>
-        <c:axId val="267939352"/>
+        <c:axId val="293570208"/>
+        <c:axId val="293570992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="267944448"/>
+        <c:axId val="293570208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +2291,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267939352"/>
+        <c:crossAx val="293570992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1656,7 +2299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="267939352"/>
+        <c:axId val="293570992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +2406,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267944448"/>
+        <c:crossAx val="293570208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1807,6 +2450,655 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scenario 2</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Increase of speed-up</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scenario2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.6325459317585298E-3"/>
+                  <c:y val="0.1072736220472441"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Scenario2!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Scenario2!$D$2:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>10.955496666963027</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.874382239276549</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.538343946553178</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.152109805159197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.848315728344382</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.553164208807244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.697223947055695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.31732388826723</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.188988001723718</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.008972946800631</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9275341997114275</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.760497132158827</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.6532094223579037</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.5508098022886045</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.4860223359492188</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.4413961462983504</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.5233557267022224</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.3995632466018204</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.5123991252345501</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.4481252658519814</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.3859589122737592</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.4398387090693898</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.4152651382745187</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.3807832064661518</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.3207502831743749</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.3130473463929793</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.3632346420327561</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.3061296083713057</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.282531051646373</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.2383149373418849</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.2075734450678937</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.3116055625227609</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="398321848"/>
+        <c:axId val="398320280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="398321848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Allocations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sv-SE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398320280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="398320280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speed-up</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sv-SE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398321848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1924,6 +3216,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2441,6 +3813,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2988,6 +5392,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3018,6 +5452,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3289,15 +5753,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3311,7 +5778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -3326,7 +5793,7 @@
         <v>1.9548087646305239</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -3341,7 +5808,7 @@
         <v>2.9313020776121794</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
@@ -3356,7 +5823,7 @@
         <v>3.6366982545995254</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>400</v>
       </c>
@@ -3371,7 +5838,7 @@
         <v>4.4329330423260771</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
@@ -3386,7 +5853,7 @@
         <v>5.1443595324410198</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>600</v>
       </c>
@@ -3401,7 +5868,7 @@
         <v>5.5462798339753139</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>700</v>
       </c>
@@ -3415,8 +5882,12 @@
         <f t="shared" si="0"/>
         <v>6.2545612032694899</v>
       </c>
+      <c r="R8">
+        <f>2.6846*LN(10000000)+0.8866*100000000000000</f>
+        <v>88660000000043.266</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>800</v>
       </c>
@@ -3431,7 +5902,7 @@
         <v>6.5821203341885832</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>900</v>
       </c>
@@ -3446,7 +5917,7 @@
         <v>6.8879555189313306</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -3461,7 +5932,7 @@
         <v>6.9246446421951866</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1100</v>
       </c>
@@ -3476,7 +5947,7 @@
         <v>6.8128678579815016</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1200</v>
       </c>
@@ -3491,7 +5962,7 @@
         <v>7.0688430058239735</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1300</v>
       </c>
@@ -3506,7 +5977,7 @@
         <v>7.2570747124257222</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1400</v>
       </c>
@@ -3521,7 +5992,7 @@
         <v>7.43906434587484</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1500</v>
       </c>
@@ -3801,8 +6272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3826,10 +6297,10 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>322.27860299999998</v>
+        <v>0.322278603</v>
       </c>
       <c r="C2">
-        <v>3530.7221610000001</v>
+        <v>3.5307221610000004</v>
       </c>
       <c r="D2">
         <f>C2/B2</f>
@@ -3841,10 +6312,10 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <v>640.94051300000001</v>
+        <v>0.64094051299999999</v>
       </c>
       <c r="C3">
-        <v>6969.8321310000001</v>
+        <v>6.9698321310000004</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D33" si="0">C3/B3</f>
@@ -3856,10 +6327,10 @@
         <v>300</v>
       </c>
       <c r="B4">
-        <v>952.16454699999997</v>
+        <v>0.95216454699999997</v>
       </c>
       <c r="C4">
-        <v>10034.23749</v>
+        <v>10.034237489999999</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -3871,10 +6342,10 @@
         <v>400</v>
       </c>
       <c r="B5">
-        <v>1271.323652</v>
+        <v>1.271323652</v>
       </c>
       <c r="C5">
-        <v>14177.940965</v>
+        <v>14.177940964999999</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -3886,14 +6357,14 @@
         <v>500</v>
       </c>
       <c r="B6">
-        <v>1569.7890190000001</v>
+        <v>1.5697890190000001</v>
       </c>
       <c r="C6">
-        <v>17029.566905</v>
+        <v>17.029566904999999</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>10.848315728344383</v>
+        <v>10.848315728344382</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3901,14 +6372,14 @@
         <v>600</v>
       </c>
       <c r="B7">
-        <v>1876.4460759999999</v>
+        <v>1.8764460759999999</v>
       </c>
       <c r="C7">
-        <v>19802.443568999999</v>
+        <v>19.802443568999998</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>10.553164208807246</v>
+        <v>10.553164208807244</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3916,10 +6387,10 @@
         <v>700</v>
       </c>
       <c r="B8">
-        <v>2227.934886</v>
+        <v>2.2279348859999999</v>
       </c>
       <c r="C8">
-        <v>23832.718414999999</v>
+        <v>23.832718414999999</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -3931,10 +6402,10 @@
         <v>800</v>
       </c>
       <c r="B9">
-        <v>2577.9281019999999</v>
+        <v>2.577928102</v>
       </c>
       <c r="C9">
-        <v>26597.319189000002</v>
+        <v>26.597319189</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -3946,14 +6417,14 @@
         <v>900</v>
       </c>
       <c r="B10">
-        <v>2846.7261629999998</v>
+        <v>2.846726163</v>
       </c>
       <c r="C10">
-        <v>29005.258719000001</v>
+        <v>29.005258719</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>10.18898800172372</v>
+        <v>10.188988001723718</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3961,10 +6432,10 @@
         <v>1000</v>
       </c>
       <c r="B11">
-        <v>3160.1835639999999</v>
+        <v>3.160183564</v>
       </c>
       <c r="C11">
-        <v>31630.191799</v>
+        <v>31.630191798999999</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -3976,10 +6447,10 @@
         <v>1100</v>
       </c>
       <c r="B12">
-        <v>3460.6497410000002</v>
+        <v>3.4606497410000001</v>
       </c>
       <c r="C12">
-        <v>34355.718656999998</v>
+        <v>34.355718656999997</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -3991,10 +6462,10 @@
         <v>1200</v>
       </c>
       <c r="B13">
-        <v>3769.5161069999999</v>
+        <v>3.7695161069999998</v>
       </c>
       <c r="C13">
-        <v>36792.351152000003</v>
+        <v>36.792351152000002</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -4006,10 +6477,10 @@
         <v>1300</v>
       </c>
       <c r="B14">
-        <v>4079.3848830000002</v>
+        <v>4.0793848830000004</v>
       </c>
       <c r="C14">
-        <v>39379.156589999999</v>
+        <v>39.379156590000001</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -4021,10 +6492,10 @@
         <v>1400</v>
       </c>
       <c r="B15">
-        <v>4404.5023090000004</v>
+        <v>4.4045023090000006</v>
       </c>
       <c r="C15">
-        <v>42066.563826999998</v>
+        <v>42.066563826999996</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -4036,10 +6507,10 @@
         <v>1500</v>
       </c>
       <c r="B16">
-        <v>4714.8362029999998</v>
+        <v>4.7148362029999999</v>
       </c>
       <c r="C16">
-        <v>44725.041532000003</v>
+        <v>44.725041532000006</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -4051,14 +6522,14 @@
         <v>1600</v>
       </c>
       <c r="B17">
-        <v>5021.0562090000003</v>
+        <v>5.0210562090000002</v>
       </c>
       <c r="C17">
-        <v>47405.780742000003</v>
+        <v>47.405780742000005</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>9.4413961462983487</v>
+        <v>9.4413961462983504</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,14 +6537,14 @@
         <v>1700</v>
       </c>
       <c r="B18">
-        <v>5325.8447740000001</v>
+        <v>5.3258447740000001</v>
       </c>
       <c r="C18">
-        <v>50719.914327999999</v>
+        <v>50.719914328000002</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>9.5233557267022206</v>
+        <v>9.5233557267022224</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4081,14 +6552,14 @@
         <v>1800</v>
       </c>
       <c r="B19">
-        <v>5666.2308990000001</v>
+        <v>5.6662308990000003</v>
       </c>
       <c r="C19">
-        <v>53260.095705</v>
+        <v>53.260095704999998</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>9.3995632466018222</v>
+        <v>9.3995632466018204</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4096,10 +6567,10 @@
         <v>1900</v>
       </c>
       <c r="B20">
-        <v>5970.7387900000003</v>
+        <v>5.9707387900000004</v>
       </c>
       <c r="C20">
-        <v>56796.050443</v>
+        <v>56.796050442999999</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -4111,10 +6582,10 @@
         <v>2000</v>
       </c>
       <c r="B21">
-        <v>6300.9404359999999</v>
+        <v>6.3009404359999994</v>
       </c>
       <c r="C21">
-        <v>59532.074531999999</v>
+        <v>59.532074531999996</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -4126,10 +6597,10 @@
         <v>2100</v>
       </c>
       <c r="B22">
-        <v>6601.0537649999997</v>
+        <v>6.6010537649999996</v>
       </c>
       <c r="C22">
-        <v>61957.219416</v>
+        <v>61.957219416000001</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -4141,14 +6612,14 @@
         <v>2200</v>
       </c>
       <c r="B23">
-        <v>6914.9762840000003</v>
+        <v>6.9149762840000006</v>
       </c>
       <c r="C23">
-        <v>65276.260798000003</v>
+        <v>65.27626079800001</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>9.439838709069388</v>
+        <v>9.4398387090693898</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4156,10 +6627,10 @@
         <v>2300</v>
       </c>
       <c r="B24">
-        <v>7219.4881839999998</v>
+        <v>7.2194881840000003</v>
       </c>
       <c r="C24">
-        <v>67973.395415000006</v>
+        <v>67.973395415000013</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -4171,10 +6642,10 @@
         <v>2400</v>
       </c>
       <c r="B25">
-        <v>7531.3216819999998</v>
+        <v>7.5313216819999997</v>
       </c>
       <c r="C25">
-        <v>70649.695957000004</v>
+        <v>70.649695957000006</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -4186,10 +6657,10 @@
         <v>2500</v>
       </c>
       <c r="B26">
-        <v>7866.3950379999997</v>
+        <v>7.8663950379999994</v>
       </c>
       <c r="C26">
-        <v>73320.703777999996</v>
+        <v>73.320703777999995</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
@@ -4201,10 +6672,10 @@
         <v>2600</v>
       </c>
       <c r="B27">
-        <v>8167.1258500000004</v>
+        <v>8.1671258499999997</v>
       </c>
       <c r="C27">
-        <v>76060.829725000003</v>
+        <v>76.060829725000005</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
@@ -4216,14 +6687,14 @@
         <v>2700</v>
       </c>
       <c r="B28">
-        <v>8484.8615339999997</v>
+        <v>8.4848615340000002</v>
       </c>
       <c r="C28">
-        <v>79445.749448000002</v>
+        <v>79.445749448000001</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>9.3632346420327579</v>
+        <v>9.3632346420327561</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4231,10 +6702,10 @@
         <v>2800</v>
       </c>
       <c r="B29">
-        <v>8800.6365060000007</v>
+        <v>8.800636506</v>
       </c>
       <c r="C29">
-        <v>81899.863960999995</v>
+        <v>81.899863960999994</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
@@ -4246,10 +6717,10 @@
         <v>2900</v>
       </c>
       <c r="B30">
-        <v>9115.8060220000007</v>
+        <v>9.115806022000001</v>
       </c>
       <c r="C30">
-        <v>84617.752460000003</v>
+        <v>84.617752460000005</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
@@ -4261,14 +6732,14 @@
         <v>3000</v>
       </c>
       <c r="B31">
-        <v>9444.2153610000005</v>
+        <v>9.4442153610000013</v>
       </c>
       <c r="C31">
-        <v>87248.635840999996</v>
+        <v>87.248635840999995</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>9.2383149373418867</v>
+        <v>9.2383149373418849</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4276,14 +6747,14 @@
         <v>3100</v>
       </c>
       <c r="B32">
-        <v>9763.7112749999997</v>
+        <v>9.7637112750000004</v>
       </c>
       <c r="C32">
-        <v>89900.088661000002</v>
+        <v>89.900088660999998</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>9.2075734450678954</v>
+        <v>9.2075734450678937</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4291,10 +6762,10 @@
         <v>3200</v>
       </c>
       <c r="B33">
-        <v>10067.381152</v>
+        <v>10.067381151999999</v>
       </c>
       <c r="C33">
-        <v>93743.482334999993</v>
+        <v>93.743482334999996</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>

</xml_diff>